<commit_message>
splitting code into functions to make it readable
</commit_message>
<xml_diff>
--- a/Partie 1 - RefSQL/Excel/Tableaux sql ref.xlsx
+++ b/Partie 1 - RefSQL/Excel/Tableaux sql ref.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ILYASS\Desktop\mission\Partie 1 - RefSQL\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ILYASS\Desktop\Stage\Mission\Partie 1 - RefSQL\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A9D97A-7CCF-49FE-9701-87194BDE64AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C817D5D1-B101-43B1-8D49-2963F51AED7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="899" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="899" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ToDO" sheetId="7" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="227">
   <si>
     <t>idSQL</t>
   </si>
@@ -275,16 +275,10 @@
     <t>coder</t>
   </si>
   <si>
-    <t>non demarree</t>
-  </si>
-  <si>
     <t>T012</t>
   </si>
   <si>
     <t>tester ; jeux de test</t>
-  </si>
-  <si>
-    <t>non demarrée</t>
   </si>
   <si>
     <t>T013</t>
@@ -808,6 +802,16 @@
   </si>
   <si>
     <t>C011</t>
+  </si>
+  <si>
+    <t>fini</t>
+  </si>
+  <si>
+    <t>les csv doivent etre placés dans le répertoire "C:\ProgramData\MySQL\MySQL Server 8.0\Data\CsvTables",</t>
+  </si>
+  <si>
+    <t>pour le moment les les tables doivent respecter le model definit dans le csv de depart               
+apres on peut generalisé les cas en important chaque collonne individuelement</t>
   </si>
 </sst>
 </file>
@@ -864,7 +868,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -919,6 +923,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -958,7 +968,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -983,6 +993,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2471,8 +2485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17497654-F13B-4E71-A230-9CAA573B118D}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,7 +2497,7 @@
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="52.7109375" customWidth="1"/>
+    <col min="7" max="7" width="96.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2533,7 +2547,7 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="F3" s="6">
         <v>45424</v>
@@ -2549,7 +2563,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="F4" s="6">
         <v>45424</v>
@@ -2565,7 +2579,7 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="F5" s="6">
         <v>45424</v>
@@ -2581,7 +2595,7 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="F6" s="6">
         <v>45424</v>
@@ -2597,7 +2611,7 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="F7" s="6">
         <v>45412</v>
@@ -2616,10 +2630,13 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="F8" s="6">
         <v>45412</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2673,11 +2690,11 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>61</v>
       </c>
@@ -2687,47 +2704,50 @@
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
       <c r="F13" s="5"/>
+      <c r="G13" s="23" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -2735,7 +2755,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2745,7 +2765,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2755,13 +2775,13 @@
     </row>
     <row r="19" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -2769,7 +2789,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2779,10 +2799,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2791,49 +2811,49 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2843,7 +2863,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2853,7 +2873,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2873,7 +2893,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D2" sqref="D2"/>
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
@@ -2927,10 +2947,10 @@
         <v>30</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="220.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2941,37 +2961,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" t="s">
         <v>194</v>
-      </c>
-      <c r="D2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E2" t="s">
-        <v>196</v>
       </c>
       <c r="F2">
         <v>202402</v>
       </c>
       <c r="G2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="M2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N2" s="21">
         <v>45385.554074074076</v>
@@ -2985,37 +3005,37 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" t="s">
         <v>194</v>
-      </c>
-      <c r="D3" t="s">
-        <v>195</v>
-      </c>
-      <c r="E3" t="s">
-        <v>196</v>
       </c>
       <c r="F3">
         <v>202402</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="M3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N3" s="21">
         <v>45385.554074074076</v>
@@ -3050,64 +3070,64 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="H2" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" s="5">
         <v>10</v>
@@ -3115,21 +3135,21 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="H3" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" s="5">
         <v>10</v>
@@ -3137,69 +3157,69 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="5">
         <v>60</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="5">
         <v>60</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="5">
         <v>60</v>
@@ -3207,72 +3227,72 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="H7" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="5">
         <v>10</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D9" s="5">
         <v>10</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="J9" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" s="5">
         <v>10</v>
@@ -3280,49 +3300,49 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="H11" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D12" s="5">
         <v>10</v>
@@ -3330,24 +3350,24 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="H12" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D13" s="5">
         <v>60</v>
@@ -3355,51 +3375,51 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="H13" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D14" s="5">
         <v>10</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D15" s="5">
         <v>10</v>
@@ -3407,103 +3427,103 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="H15" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="H16" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D17" s="5">
         <v>60</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D18" s="5">
         <v>60</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>120</v>
-      </c>
       <c r="I18" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D19" s="5">
         <v>60</v>
@@ -3511,76 +3531,76 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="H19" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D20" s="5">
         <v>10</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="H21" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D22" s="5">
         <v>10</v>
@@ -3588,24 +3608,24 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="H22" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D23" s="5">
         <v>10</v>
@@ -3613,24 +3633,24 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D24" s="5">
         <v>1000</v>
@@ -3638,49 +3658,49 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="H24" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="H25" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D26" s="5">
         <v>200</v>
@@ -3688,24 +3708,24 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="H26" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D27" s="5">
         <v>200</v>
@@ -3713,24 +3733,24 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="H27" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D28" s="5">
         <v>200</v>
@@ -3738,24 +3758,24 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D29" s="5">
         <v>200</v>
@@ -3763,99 +3783,99 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="H30" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="H31" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="H32" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D33" s="5">
         <v>10</v>
@@ -3863,74 +3883,74 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="H33" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="H34" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="H35" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D36" s="5">
         <v>10</v>
@@ -3938,24 +3958,24 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="H36" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D37" s="5">
         <v>10</v>
@@ -3963,76 +3983,76 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="H37" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D38" s="5">
         <v>10</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D41" s="5">
         <v>200</v>
@@ -4042,13 +4062,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D42" s="5">
         <v>200</v>
@@ -4058,13 +4078,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D43" s="5">
         <v>200</v>
@@ -4074,13 +4094,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D44" s="5">
         <v>10</v>
@@ -4090,31 +4110,31 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D45" s="5">
         <v>10</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D46" s="5">
         <v>10</v>
@@ -4124,13 +4144,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D47" s="5">
         <v>10</v>
@@ -4140,13 +4160,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D48" s="5">
         <v>10</v>
@@ -4156,13 +4176,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D49" s="5">
         <v>1000</v>
@@ -4172,13 +4192,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D50" s="5">
         <v>1000</v>
@@ -4248,13 +4268,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>169</v>
-      </c>
-      <c r="C2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -4262,13 +4282,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="C3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -4318,16 +4338,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" t="s">
         <v>194</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>195</v>
-      </c>
-      <c r="D2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4335,16 +4355,16 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" t="s">
         <v>198</v>
-      </c>
-      <c r="D3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4352,16 +4372,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
         <v>205</v>
-      </c>
-      <c r="C4" t="s">
-        <v>206</v>
-      </c>
-      <c r="D4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -4407,53 +4427,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C2" s="17">
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C3" s="17">
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C4" s="17">
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -4524,303 +4544,303 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C2" s="17">
         <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H2" s="19">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C3" s="17">
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H3" s="19">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C4" s="17">
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H4" s="19">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C5" s="17">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H5" s="19">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J5" t="s">
+        <v>181</v>
+      </c>
+      <c r="K5" t="s">
         <v>183</v>
       </c>
-      <c r="K5" t="s">
-        <v>185</v>
-      </c>
       <c r="L5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C6" s="17">
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H6" s="19">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K6" t="s">
+        <v>184</v>
+      </c>
+      <c r="L6" t="s">
         <v>186</v>
-      </c>
-      <c r="L6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="17">
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H7" s="19">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C8" s="17">
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H8" s="19">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C9" s="17">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H9" s="19">
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -4856,7 +4876,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -4870,7 +4890,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4881,7 +4901,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4892,7 +4912,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4903,7 +4923,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -4940,7 +4960,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -4969,22 +4989,22 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s">
         <v>189</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" t="s">
         <v>191</v>
-      </c>
-      <c r="E2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" t="s">
-        <v>193</v>
       </c>
       <c r="G2">
         <v>14015</v>
       </c>
       <c r="H2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4995,22 +5015,22 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G3">
         <v>17515</v>
       </c>
       <c r="H3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5021,22 +5041,22 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
         <v>190</v>
       </c>
-      <c r="D4" t="s">
-        <v>192</v>
-      </c>
       <c r="E4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G4">
         <v>11315</v>
       </c>
       <c r="H4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5047,22 +5067,22 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" t="s">
         <v>190</v>
       </c>
-      <c r="D5" t="s">
-        <v>192</v>
-      </c>
       <c r="E5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G5">
         <v>11315</v>
       </c>
       <c r="H5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -5097,13 +5117,13 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" t="s">
         <v>217</v>
-      </c>
-      <c r="D1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5111,16 +5131,16 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5128,16 +5148,16 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5145,16 +5165,16 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -5220,7 +5240,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E2" s="19">
         <v>28</v>
@@ -5229,13 +5249,13 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5249,7 +5269,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E3" s="19">
         <v>28</v>
@@ -5258,13 +5278,13 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5278,7 +5298,7 @@
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E4" s="17">
         <v>30</v>
@@ -5287,13 +5307,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5307,7 +5327,7 @@
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E5" s="17">
         <v>29</v>
@@ -5316,13 +5336,13 @@
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>